<commit_message>
Add Test to Edit not exist entity
</commit_message>
<xml_diff>
--- a/TestData/Data/Repports/SanctionCategory.xlsx
+++ b/TestData/Data/Repports/SanctionCategory.xlsx
@@ -22,52 +22,52 @@
     <x:t>MessageType</x:t>
   </x:si>
   <x:si>
-    <x:t>Insertion de l'entity 1ère mise en garde</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Add_Success</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity 2ème mise en garde</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity 1er avertissement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity 2ème avertissement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Blâme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion de 2 jours</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion temporaire ou définitive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion temporaire ou définitive_8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion temporaire ou définitive_9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion définitive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Mise en Garde Comportement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Avertissement_Comportement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Blâme_Comportement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion de 2 jours Comportement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Insertion de l'entity Exclusion définitive Comportement</x:t>
+    <x:t>Mise à jour de l'entity 1ère mise en garde</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Update_Success</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity 2ème mise en garde</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity 1er avertissement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity 2ème avertissement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Blâme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion de 2 jours</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion temporaire ou définitive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion temporaire ou définitive_8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion temporaire ou définitive_9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion définitive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Mise en Garde Comportement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Avertissement_Comportement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Blâme_Comportement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion de 2 jours Comportement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mise à jour de l'entity Exclusion définitive Comportement</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -435,7 +435,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="50.200625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="52.110625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="16.175425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>